<commit_message>
Informe final de la tercera fase de desarrollo del Sprint
</commit_message>
<xml_diff>
--- a/Product backlog y calendarización.xlsx
+++ b/Product backlog y calendarización.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1c7720fd83b1034c/Documentos/LDSW/SEGUNDO SEMESTRE/Proyecto II/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{36156E1A-6B95-48A6-A4D8-D3D6B0A75CD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{36156E1A-6B95-48A6-A4D8-D3D6B0A75CD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{99B3719A-B264-4E35-9F89-C84975DFA0C2}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2088" yWindow="2088" windowWidth="2388" windowHeight="564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Estimación de esfuerzo" sheetId="1" r:id="rId1"/>
@@ -361,16 +361,16 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
+        <top style="thin">
           <color auto="1"/>
-        </bottom>
+        </top>
       </border>
     </dxf>
     <dxf>
       <border outline="0">
-        <top style="thin">
+        <bottom style="thin">
           <color auto="1"/>
-        </top>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -404,16 +404,16 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
+        <top style="thin">
           <color auto="1"/>
-        </bottom>
+        </top>
       </border>
     </dxf>
     <dxf>
       <border outline="0">
-        <top style="thin">
+        <bottom style="thin">
           <color auto="1"/>
-        </top>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -459,7 +459,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{75010DB0-A5DF-4AA2-9F9C-5803D488BE68}" name="Tabla1" displayName="Tabla1" ref="A1:F31" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="4" tableBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{75010DB0-A5DF-4AA2-9F9C-5803D488BE68}" name="Tabla1" displayName="Tabla1" ref="A1:F31" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4">
   <autoFilter ref="A1:F31" xr:uid="{75010DB0-A5DF-4AA2-9F9C-5803D488BE68}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{5E9FF93A-7310-4B2D-820D-7259811C6BF2}" name="Historia de Usuario"/>
@@ -474,8 +474,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E15392DE-307A-4AC1-86B6-CCC975116024}" name="Tabla13" displayName="Tabla13" ref="A35:D40" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="1" tableBorderDxfId="2">
-  <autoFilter ref="A35:D40" xr:uid="{D856270B-60E1-4990-9936-4112B16A1CD6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E15392DE-307A-4AC1-86B6-CCC975116024}" name="Tabla13" displayName="Tabla13" ref="A35:D40" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1">
+  <autoFilter ref="A35:D40" xr:uid="{D856270B-60E1-4990-9936-4112B16A1CD6}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+  </autoFilter>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{CDF4F3BF-DF3A-457A-BA79-013B87E250C2}" name="Sprint" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{BB7E669B-8A77-4DFA-BDFA-4A56C86EB147}" name="Fecha de Inicio"/>
@@ -775,8 +780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>